<commit_message>
message after adding filter s
</commit_message>
<xml_diff>
--- a/EXCEL1.xlsx
+++ b/EXCEL1.xlsx
@@ -17,6 +17,8 @@
     <x:sheet name="amex_26-12-2024" sheetId="5" r:id="rId5"/>
     <x:sheet name="amex_27-12-2024" sheetId="6" r:id="rId6"/>
     <x:sheet name="bof_27-12-2024" sheetId="7" r:id="rId7"/>
+    <x:sheet name="amex_28-12-2024" sheetId="8" r:id="rId8"/>
+    <x:sheet name="bof_28-12-2024" sheetId="9" r:id="rId9"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="162913"/>
@@ -1808,6 +1810,81 @@
   </x:si>
   <x:si>
     <x:t>Exp. 01/25/25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>honeylove</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.aexp-static.com/amexoffers/images/logos/00P5b00001l7oevEAA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>intimissimi</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.aexp-static.com/amexoffers/images/logos/00P5b00001l7ocuEAA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>origins</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.aexp-static.com/amexoffers/images/logos/00P5b00001l7odTEAQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Big Sky Resort- Montana</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.aexp-static.com/amexoffers/images/logos/00P5b00001l7jsaEAA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>03/22/2025</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jbl</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.aexp-static.com/amexoffers/images/logos/00P5b00001l7lCwEAI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Earn 10% back on purchases, up to a total of $250</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Expires in 11 days</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Expires tomorrow</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AncestryDNA® Kits</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.aexp-static.com/amexoffers/images/logos/00P5b00001l7ntHEAQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Earn 20% back on a single purchase, up to a total of $70</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jenni Kayne - Apparel &amp; Home Essentials</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.aexp-static.com/amexoffers/images/logos/00P5b00001CiXnzEAF</x:t>
+  </x:si>
+  <x:si>
+    <x:t>canon</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.aexp-static.com/amexoffers/images/logos/00P5b00001l7ocpEAA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Omni Hotels &amp; Resorts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.aexp-static.com/amexoffers/images/logos/00P5b00001l7NKHEA2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Spend $750 or more, earn $150 back. Enroll by 2/20/2025.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>03/20/2025</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -7812,4 +7889,2858 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:D100"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>259</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>265</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="0" t="s">
+        <x:v>283</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>286</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="0" t="s">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>273</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>275</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="A5" s="0" t="s">
+        <x:v>295</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>296</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="A6" s="0" t="s">
+        <x:v>276</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>277</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>279</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4">
+      <x:c r="A7" s="0" t="s">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>288</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>289</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>290</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="A8" s="0" t="s">
+        <x:v>361</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>362</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="A9" s="0" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>321</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="A10" s="0" t="s">
+        <x:v>378</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>379</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>380</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:4">
+      <x:c r="A11" s="0" t="s">
+        <x:v>390</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>391</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>392</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>393</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="A12" s="0" t="s">
+        <x:v>322</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>323</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="A13" s="0" t="s">
+        <x:v>336</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>308</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="A14" s="0" t="s">
+        <x:v>329</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>330</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>314</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="A15" s="0" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>310</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="A16" s="0" t="s">
+        <x:v>280</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>275</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="A17" s="0" t="s">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>385</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>386</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:4">
+      <x:c r="A18" s="0" t="s">
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>306</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>307</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>308</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="A19" s="0" t="s">
+        <x:v>368</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>369</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="A20" s="0" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:4">
+      <x:c r="A21" s="0" t="s">
+        <x:v>366</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>367</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:4">
+      <x:c r="A22" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>263</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="A23" s="0" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>347</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>349</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4">
+      <x:c r="A24" s="0" t="s">
+        <x:v>331</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>332</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:4">
+      <x:c r="A25" s="0" t="s">
+        <x:v>316</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>317</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>318</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>319</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="A26" s="0" t="s">
+        <x:v>445</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>446</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="A27" s="0" t="s">
+        <x:v>357</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>358</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>359</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>360</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4">
+      <x:c r="A28" s="0" t="s">
+        <x:v>325</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>327</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>271</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="A29" s="0" t="s">
+        <x:v>343</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>345</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>290</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="A30" s="0" t="s">
+        <x:v>447</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:4">
+      <x:c r="A31" s="0" t="s">
+        <x:v>407</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>408</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>409</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="A32" s="0" t="s">
+        <x:v>298</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>299</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4">
+      <x:c r="A33" s="0" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>351</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>353</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:4">
+      <x:c r="A34" s="0" t="s">
+        <x:v>397</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>398</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>399</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>400</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:4">
+      <x:c r="A35" s="0" t="s">
+        <x:v>363</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>365</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>360</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:4">
+      <x:c r="A36" s="0" t="s">
+        <x:v>302</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>303</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:4">
+      <x:c r="A37" s="0" t="s">
+        <x:v>467</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:4">
+      <x:c r="A38" s="0" t="s">
+        <x:v>436</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>437</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:4">
+      <x:c r="A39" s="0" t="s">
+        <x:v>488</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>489</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:4">
+      <x:c r="A40" s="0" t="s">
+        <x:v>333</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>334</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>335</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:4">
+      <x:c r="A41" s="0" t="s">
+        <x:v>486</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>487</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:4">
+      <x:c r="A42" s="0" t="s">
+        <x:v>410</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>411</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>341</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>412</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:4">
+      <x:c r="A43" s="0" t="s">
+        <x:v>376</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>377</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>341</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:4">
+      <x:c r="A44" s="0" t="s">
+        <x:v>494</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>495</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>496</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>308</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:4">
+      <x:c r="A45" s="0" t="s">
+        <x:v>558</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>559</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>560</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:4">
+      <x:c r="A46" s="0" t="s">
+        <x:v>387</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>388</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>389</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:4">
+      <x:c r="A47" s="0" t="s">
+        <x:v>492</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>493</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:4">
+      <x:c r="A48" s="0" t="s">
+        <x:v>451</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>392</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="s">
+        <x:v>453</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:4">
+      <x:c r="A49" s="0" t="s">
+        <x:v>339</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>341</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>342</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:4">
+      <x:c r="A50" s="0" t="s">
+        <x:v>490</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>491</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:4">
+      <x:c r="A51" s="0" t="s">
+        <x:v>530</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>531</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:4">
+      <x:c r="A52" s="0" t="s">
+        <x:v>423</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>424</x:v>
+      </x:c>
+      <x:c r="C52" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="D52" s="0" t="s">
+        <x:v>308</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:4">
+      <x:c r="A53" s="0" t="s">
+        <x:v>429</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>430</x:v>
+      </x:c>
+      <x:c r="C53" s="0" t="s">
+        <x:v>431</x:v>
+      </x:c>
+      <x:c r="D53" s="0" t="s">
+        <x:v>432</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:4">
+      <x:c r="A54" s="0" t="s">
+        <x:v>587</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>588</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="s">
+        <x:v>484</x:v>
+      </x:c>
+      <x:c r="D54" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:4">
+      <x:c r="A55" s="0" t="s">
+        <x:v>459</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>460</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D55" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:4">
+      <x:c r="A56" s="0" t="s">
+        <x:v>480</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>481</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="D56" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:4">
+      <x:c r="A57" s="0" t="s">
+        <x:v>420</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>421</x:v>
+      </x:c>
+      <x:c r="C57" s="0" t="s">
+        <x:v>422</x:v>
+      </x:c>
+      <x:c r="D57" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:4">
+      <x:c r="A58" s="0" t="s">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>441</x:v>
+      </x:c>
+      <x:c r="C58" s="0" t="s">
+        <x:v>442</x:v>
+      </x:c>
+      <x:c r="D58" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:4">
+      <x:c r="A59" s="0" t="s">
+        <x:v>463</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>464</x:v>
+      </x:c>
+      <x:c r="C59" s="0" t="s">
+        <x:v>465</x:v>
+      </x:c>
+      <x:c r="D59" s="0" t="s">
+        <x:v>466</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:4">
+      <x:c r="A60" s="0" t="s">
+        <x:v>394</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>395</x:v>
+      </x:c>
+      <x:c r="C60" s="0" t="s">
+        <x:v>396</x:v>
+      </x:c>
+      <x:c r="D60" s="0" t="s">
+        <x:v>360</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:4">
+      <x:c r="A61" s="0" t="s">
+        <x:v>516</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>517</x:v>
+      </x:c>
+      <x:c r="C61" s="0" t="s">
+        <x:v>422</x:v>
+      </x:c>
+      <x:c r="D61" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:4">
+      <x:c r="A62" s="0" t="s">
+        <x:v>449</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>450</x:v>
+      </x:c>
+      <x:c r="C62" s="0" t="s">
+        <x:v>386</x:v>
+      </x:c>
+      <x:c r="D62" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:4">
+      <x:c r="A63" s="0" t="s">
+        <x:v>534</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>535</x:v>
+      </x:c>
+      <x:c r="C63" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D63" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:4">
+      <x:c r="A64" s="0" t="s">
+        <x:v>454</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>455</x:v>
+      </x:c>
+      <x:c r="C64" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="D64" s="0" t="s">
+        <x:v>456</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:4">
+      <x:c r="A65" s="0" t="s">
+        <x:v>556</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>557</x:v>
+      </x:c>
+      <x:c r="C65" s="0" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="D65" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:4">
+      <x:c r="A66" s="0" t="s">
+        <x:v>593</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>594</x:v>
+      </x:c>
+      <x:c r="C66" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D66" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:4">
+      <x:c r="A67" s="0" t="s">
+        <x:v>443</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>444</x:v>
+      </x:c>
+      <x:c r="C67" s="0" t="s">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="D67" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:4">
+      <x:c r="A68" s="0" t="s">
+        <x:v>401</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>402</x:v>
+      </x:c>
+      <x:c r="C68" s="0" t="s">
+        <x:v>403</x:v>
+      </x:c>
+      <x:c r="D68" s="0" t="s">
+        <x:v>404</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:4">
+      <x:c r="A69" s="0" t="s">
+        <x:v>518</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>519</x:v>
+      </x:c>
+      <x:c r="C69" s="0" t="s">
+        <x:v>520</x:v>
+      </x:c>
+      <x:c r="D69" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:4">
+      <x:c r="A70" s="0" t="s">
+        <x:v>574</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>575</x:v>
+      </x:c>
+      <x:c r="C70" s="0" t="s">
+        <x:v>386</x:v>
+      </x:c>
+      <x:c r="D70" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:4">
+      <x:c r="A71" s="0" t="s">
+        <x:v>405</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>406</x:v>
+      </x:c>
+      <x:c r="C71" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="D71" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:4">
+      <x:c r="A72" s="0" t="s">
+        <x:v>536</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>537</x:v>
+      </x:c>
+      <x:c r="C72" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="D72" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:4">
+      <x:c r="A73" s="0" t="s">
+        <x:v>525</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>526</x:v>
+      </x:c>
+      <x:c r="C73" s="0" t="s">
+        <x:v>527</x:v>
+      </x:c>
+      <x:c r="D73" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:4">
+      <x:c r="A74" s="0" t="s">
+        <x:v>501</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>502</x:v>
+      </x:c>
+      <x:c r="C74" s="0" t="s">
+        <x:v>503</x:v>
+      </x:c>
+      <x:c r="D74" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:4">
+      <x:c r="A75" s="0" t="s">
+        <x:v>581</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>582</x:v>
+      </x:c>
+      <x:c r="C75" s="0" t="s">
+        <x:v>583</x:v>
+      </x:c>
+      <x:c r="D75" s="0" t="s">
+        <x:v>573</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:4">
+      <x:c r="A76" s="0" t="s">
+        <x:v>595</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>596</x:v>
+      </x:c>
+      <x:c r="C76" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="D76" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:4">
+      <x:c r="A77" s="0" t="s">
+        <x:v>528</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>529</x:v>
+      </x:c>
+      <x:c r="C77" s="0" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="D77" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:4">
+      <x:c r="A78" s="0" t="s">
+        <x:v>562</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>563</x:v>
+      </x:c>
+      <x:c r="C78" s="0" t="s">
+        <x:v>392</x:v>
+      </x:c>
+      <x:c r="D78" s="0" t="s">
+        <x:v>564</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:4">
+      <x:c r="A79" s="0" t="s">
+        <x:v>482</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>483</x:v>
+      </x:c>
+      <x:c r="C79" s="0" t="s">
+        <x:v>484</x:v>
+      </x:c>
+      <x:c r="D79" s="0" t="s">
+        <x:v>485</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:4">
+      <x:c r="A80" s="0" t="s">
+        <x:v>473</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
+        <x:v>474</x:v>
+      </x:c>
+      <x:c r="C80" s="0" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="D80" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:4">
+      <x:c r="A81" s="0" t="s">
+        <x:v>457</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
+        <x:v>458</x:v>
+      </x:c>
+      <x:c r="C81" s="0" t="s">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="D81" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:4">
+      <x:c r="A82" s="0" t="s">
+        <x:v>552</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
+        <x:v>553</x:v>
+      </x:c>
+      <x:c r="C82" s="0" t="s">
+        <x:v>554</x:v>
+      </x:c>
+      <x:c r="D82" s="0" t="s">
+        <x:v>555</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:4">
+      <x:c r="A83" s="0" t="s">
+        <x:v>576</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>577</x:v>
+      </x:c>
+      <x:c r="C83" s="0" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="D83" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:4">
+      <x:c r="A84" s="0" t="s">
+        <x:v>370</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
+        <x:v>371</x:v>
+      </x:c>
+      <x:c r="C84" s="0" t="s">
+        <x:v>372</x:v>
+      </x:c>
+      <x:c r="D84" s="0" t="s">
+        <x:v>373</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:4">
+      <x:c r="A85" s="0" t="s">
+        <x:v>597</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>598</x:v>
+      </x:c>
+      <x:c r="C85" s="0" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="D85" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:4">
+      <x:c r="A86" s="0" t="s">
+        <x:v>599</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>600</x:v>
+      </x:c>
+      <x:c r="C86" s="0" t="s">
+        <x:v>392</x:v>
+      </x:c>
+      <x:c r="D86" s="0" t="s">
+        <x:v>601</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:4">
+      <x:c r="A87" s="0" t="s">
+        <x:v>425</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
+        <x:v>426</x:v>
+      </x:c>
+      <x:c r="C87" s="0" t="s">
+        <x:v>427</x:v>
+      </x:c>
+      <x:c r="D87" s="0" t="s">
+        <x:v>328</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:4">
+      <x:c r="A88" s="0" t="s">
+        <x:v>565</x:v>
+      </x:c>
+      <x:c r="B88" s="0" t="s">
+        <x:v>566</x:v>
+      </x:c>
+      <x:c r="C88" s="0" t="s">
+        <x:v>314</x:v>
+      </x:c>
+      <x:c r="D88" s="0" t="s">
+        <x:v>567</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:4">
+      <x:c r="A89" s="0" t="s">
+        <x:v>475</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
+        <x:v>476</x:v>
+      </x:c>
+      <x:c r="C89" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D89" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:4">
+      <x:c r="A90" s="0" t="s">
+        <x:v>504</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>505</x:v>
+      </x:c>
+      <x:c r="C90" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D90" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:4">
+      <x:c r="A91" s="0" t="s">
+        <x:v>538</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>539</x:v>
+      </x:c>
+      <x:c r="C91" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D91" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:4">
+      <x:c r="A92" s="0" t="s">
+        <x:v>602</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>603</x:v>
+      </x:c>
+      <x:c r="C92" s="0" t="s">
+        <x:v>604</x:v>
+      </x:c>
+      <x:c r="D92" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:4">
+      <x:c r="A93" s="0" t="s">
+        <x:v>548</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>549</x:v>
+      </x:c>
+      <x:c r="C93" s="0" t="s">
+        <x:v>550</x:v>
+      </x:c>
+      <x:c r="D93" s="0" t="s">
+        <x:v>605</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:4">
+      <x:c r="A94" s="0" t="s">
+        <x:v>413</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>414</x:v>
+      </x:c>
+      <x:c r="C94" s="0" t="s">
+        <x:v>415</x:v>
+      </x:c>
+      <x:c r="D94" s="0" t="s">
+        <x:v>606</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:4">
+      <x:c r="A95" s="0" t="s">
+        <x:v>607</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>608</x:v>
+      </x:c>
+      <x:c r="C95" s="0" t="s">
+        <x:v>609</x:v>
+      </x:c>
+      <x:c r="D95" s="0" t="s">
+        <x:v>400</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:4">
+      <x:c r="A96" s="0" t="s">
+        <x:v>374</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>375</x:v>
+      </x:c>
+      <x:c r="C96" s="0" t="s">
+        <x:v>314</x:v>
+      </x:c>
+      <x:c r="D96" s="0" t="s">
+        <x:v>286</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:4">
+      <x:c r="A97" s="0" t="s">
+        <x:v>610</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>611</x:v>
+      </x:c>
+      <x:c r="C97" s="0" t="s">
+        <x:v>327</x:v>
+      </x:c>
+      <x:c r="D97" s="0" t="s">
+        <x:v>564</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:4">
+      <x:c r="A98" s="0" t="s">
+        <x:v>612</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>613</x:v>
+      </x:c>
+      <x:c r="C98" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="D98" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:4">
+      <x:c r="A99" s="0" t="s">
+        <x:v>614</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>615</x:v>
+      </x:c>
+      <x:c r="C99" s="0" t="s">
+        <x:v>616</x:v>
+      </x:c>
+      <x:c r="D99" s="0" t="s">
+        <x:v>617</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:4">
+      <x:c r="A100" s="0" t="s">
+        <x:v>497</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>498</x:v>
+      </x:c>
+      <x:c r="C100" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="D100" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:D101"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="A5" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="A6" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4">
+      <x:c r="A7" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="A8" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="A9" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="A10" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:4">
+      <x:c r="A11" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="A12" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="A13" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="A14" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="A15" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="A16" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="A17" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:4">
+      <x:c r="A18" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="A19" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="A20" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:4">
+      <x:c r="A21" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:4">
+      <x:c r="A22" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="A23" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4">
+      <x:c r="A24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:4">
+      <x:c r="A25" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="A26" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="A27" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4">
+      <x:c r="A28" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="A29" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="A30" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:4">
+      <x:c r="A31" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="A32" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4">
+      <x:c r="A33" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:4">
+      <x:c r="A34" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:4">
+      <x:c r="A35" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:4">
+      <x:c r="A36" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:4">
+      <x:c r="A37" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:4">
+      <x:c r="A38" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:4">
+      <x:c r="A39" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:4">
+      <x:c r="A40" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:4">
+      <x:c r="A41" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:4">
+      <x:c r="A42" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:4">
+      <x:c r="A43" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:4">
+      <x:c r="A44" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:4">
+      <x:c r="A45" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:4">
+      <x:c r="A46" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:4">
+      <x:c r="A47" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:4">
+      <x:c r="A48" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:4">
+      <x:c r="A49" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:4">
+      <x:c r="A50" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:4">
+      <x:c r="A51" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:4">
+      <x:c r="A52" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="C52" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D52" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:4">
+      <x:c r="A53" s="0" t="s">
+        <x:v>149</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="C53" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="D53" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:4">
+      <x:c r="A54" s="0" t="s">
+        <x:v>151</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D54" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:4">
+      <x:c r="A55" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D55" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:4">
+      <x:c r="A56" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D56" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:4">
+      <x:c r="A57" s="0" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="C57" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="D57" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:4">
+      <x:c r="A58" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="C58" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D58" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:4">
+      <x:c r="A59" s="0" t="s">
+        <x:v>161</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="C59" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D59" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:4">
+      <x:c r="A60" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="C60" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D60" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:4">
+      <x:c r="A61" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="C61" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D61" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:4">
+      <x:c r="A62" s="0" t="s">
+        <x:v>167</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="C62" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D62" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:4">
+      <x:c r="A63" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C63" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D63" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:4">
+      <x:c r="A64" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="C64" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D64" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:4">
+      <x:c r="A65" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="C65" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="D65" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:4">
+      <x:c r="A66" s="0" t="s">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>174</x:v>
+      </x:c>
+      <x:c r="C66" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D66" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:4">
+      <x:c r="A67" s="0" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>176</x:v>
+      </x:c>
+      <x:c r="C67" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D67" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:4">
+      <x:c r="A68" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>178</x:v>
+      </x:c>
+      <x:c r="C68" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="D68" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:4">
+      <x:c r="A69" s="0" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="C69" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="D69" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:4">
+      <x:c r="A70" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="C70" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D70" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:4">
+      <x:c r="A71" s="0" t="s">
+        <x:v>183</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>184</x:v>
+      </x:c>
+      <x:c r="C71" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D71" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:4">
+      <x:c r="A72" s="0" t="s">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="C72" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="D72" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:4">
+      <x:c r="A73" s="0" t="s">
+        <x:v>187</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="C73" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D73" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:4">
+      <x:c r="A74" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="C74" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="D74" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:4">
+      <x:c r="A75" s="0" t="s">
+        <x:v>191</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>192</x:v>
+      </x:c>
+      <x:c r="C75" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D75" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:4">
+      <x:c r="A76" s="0" t="s">
+        <x:v>193</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>194</x:v>
+      </x:c>
+      <x:c r="C76" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="D76" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:4">
+      <x:c r="A77" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>196</x:v>
+      </x:c>
+      <x:c r="C77" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D77" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:4">
+      <x:c r="A78" s="0" t="s">
+        <x:v>197</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>198</x:v>
+      </x:c>
+      <x:c r="C78" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D78" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:4">
+      <x:c r="A79" s="0" t="s">
+        <x:v>199</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="C79" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="D79" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:4">
+      <x:c r="A80" s="0" t="s">
+        <x:v>201</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="C80" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D80" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:4">
+      <x:c r="A81" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="C81" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D81" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:4">
+      <x:c r="A82" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
+        <x:v>206</x:v>
+      </x:c>
+      <x:c r="C82" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D82" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:4">
+      <x:c r="A83" s="0" t="s">
+        <x:v>207</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>208</x:v>
+      </x:c>
+      <x:c r="C83" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D83" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:4">
+      <x:c r="A84" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="C84" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="D84" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:4">
+      <x:c r="A85" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>212</x:v>
+      </x:c>
+      <x:c r="C85" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D85" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:4">
+      <x:c r="A86" s="0" t="s">
+        <x:v>213</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="C86" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D86" s="0" t="s">
+        <x:v>215</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:4">
+      <x:c r="A87" s="0" t="s">
+        <x:v>216</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
+        <x:v>217</x:v>
+      </x:c>
+      <x:c r="C87" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D87" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:4">
+      <x:c r="A88" s="0" t="s">
+        <x:v>218</x:v>
+      </x:c>
+      <x:c r="B88" s="0" t="s">
+        <x:v>219</x:v>
+      </x:c>
+      <x:c r="C88" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D88" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:4">
+      <x:c r="A89" s="0" t="s">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+      <x:c r="C89" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="D89" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:4">
+      <x:c r="A90" s="0" t="s">
+        <x:v>223</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>224</x:v>
+      </x:c>
+      <x:c r="C90" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D90" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:4">
+      <x:c r="A91" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+      <x:c r="C91" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="D91" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:4">
+      <x:c r="A92" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+      <x:c r="C92" s="0" t="s">
+        <x:v>229</x:v>
+      </x:c>
+      <x:c r="D92" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:4">
+      <x:c r="A93" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
+      <x:c r="C93" s="0" t="s">
+        <x:v>232</x:v>
+      </x:c>
+      <x:c r="D93" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:4">
+      <x:c r="A94" s="0" t="s">
+        <x:v>237</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>238</x:v>
+      </x:c>
+      <x:c r="C94" s="0" t="s">
+        <x:v>239</x:v>
+      </x:c>
+      <x:c r="D94" s="0" t="s">
+        <x:v>235</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:4">
+      <x:c r="A95" s="0" t="s">
+        <x:v>233</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>234</x:v>
+      </x:c>
+      <x:c r="C95" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="D95" s="0" t="s">
+        <x:v>235</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:4">
+      <x:c r="A96" s="0" t="s">
+        <x:v>240</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>241</x:v>
+      </x:c>
+      <x:c r="C96" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D96" s="0" t="s">
+        <x:v>242</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:4">
+      <x:c r="A97" s="0" t="s">
+        <x:v>243</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>244</x:v>
+      </x:c>
+      <x:c r="C97" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D97" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:4">
+      <x:c r="A98" s="0" t="s">
+        <x:v>245</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>246</x:v>
+      </x:c>
+      <x:c r="C98" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D98" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:4">
+      <x:c r="A99" s="0" t="s">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+      <x:c r="C99" s="0" t="s">
+        <x:v>252</x:v>
+      </x:c>
+      <x:c r="D99" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:4">
+      <x:c r="A100" s="0" t="s">
+        <x:v>247</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>248</x:v>
+      </x:c>
+      <x:c r="C100" s="0" t="s">
+        <x:v>249</x:v>
+      </x:c>
+      <x:c r="D100" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:4">
+      <x:c r="A101" s="0" t="s">
+        <x:v>253</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>254</x:v>
+      </x:c>
+      <x:c r="C101" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="D101" s="0" t="s">
+        <x:v>255</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>